<commit_message>
Added some more validation
</commit_message>
<xml_diff>
--- a/config/acc_rem.xlsx
+++ b/config/acc_rem.xlsx
@@ -436,7 +436,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -470,16 +470,16 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -816,7 +816,7 @@
     <col min="12" max="12" style="7" width="29.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -946,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -978,7 +978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1312,7 +1312,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>